<commit_message>
BOM bug, LED resistor to 270R
</commit_message>
<xml_diff>
--- a/bom/BOM.xlsx
+++ b/bom/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\KiCad\HWmonitor_DSPlink\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A38599-7108-4C9E-8E15-E2BD63F7F041}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA68908-15E5-4885-B7F3-43DAA5772997}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8445" yWindow="3360" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="by MPNs" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="238">
   <si>
     <t/>
   </si>
@@ -691,15 +691,9 @@
     <t>14</t>
   </si>
   <si>
-    <t>R1, R2, R4, R5, R6, R7, R11, R12, R13, R14, R23, R24, R25, R26</t>
-  </si>
-  <si>
     <t>15</t>
   </si>
   <si>
-    <t>R8, R9</t>
-  </si>
-  <si>
     <t>16</t>
   </si>
   <si>
@@ -755,6 +749,12 @@
   </si>
   <si>
     <t>131-3701-301 OR 731000103</t>
+  </si>
+  <si>
+    <t>R1, R2, R5, R6, R7, R11, R12, R13, R14, R23, R24, R25, R26</t>
+  </si>
+  <si>
+    <t>R4, R8, R9</t>
   </si>
 </sst>
 </file>
@@ -790,9 +790,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1181,7 +1184,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1285,7 +1288,7 @@
         <v>201</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>11</v>
@@ -1297,7 +1300,7 @@
         <v>13</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1536,11 +1539,11 @@
       <c r="A14" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>215</v>
+      <c r="B14" s="2">
+        <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>216</v>
+        <v>236</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>104</v>
@@ -1586,13 +1589,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>196</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>218</v>
+        <v>237</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>115</v>
@@ -1612,7 +1615,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>193</v>
@@ -1638,13 +1641,13 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>207</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>124</v>
@@ -1664,13 +1667,13 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>196</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>137</v>
@@ -1690,7 +1693,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>193</v>
@@ -1716,7 +1719,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>193</v>
@@ -1742,7 +1745,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>193</v>
@@ -1794,7 +1797,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>193</v>
@@ -1820,7 +1823,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>193</v>
@@ -1846,7 +1849,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>193</v>
@@ -1872,7 +1875,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>193</v>
@@ -1898,13 +1901,13 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>200</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>172</v>
@@ -1924,7 +1927,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>193</v>
@@ -1950,13 +1953,13 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>200</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>185</v>
@@ -1971,7 +1974,7 @@
         <v>188</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>